<commit_message>
Added usage notes to test plan
</commit_message>
<xml_diff>
--- a/test_files/ServiceTestMatrix.xlsx
+++ b/test_files/ServiceTestMatrix.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="5400" windowWidth="25485" windowHeight="11220"/>
+    <workbookView xWindow="1815" yWindow="5460" windowWidth="25485" windowHeight="11160" tabRatio="318"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t>Endpoint</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>sessionId must be a valid ID (This changes with each session)</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,6 +721,9 @@
       <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -747,6 +753,9 @@
       <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -775,6 +784,9 @@
       <c r="I5" s="3">
         <v>41507</v>
       </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -803,6 +815,9 @@
       <c r="I6" s="3">
         <v>41507</v>
       </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -831,6 +846,9 @@
       <c r="I7" s="3">
         <v>41507</v>
       </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -859,6 +877,9 @@
       <c r="I8" s="3">
         <v>41507</v>
       </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -887,6 +908,9 @@
       <c r="I9" s="3">
         <v>41507</v>
       </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -915,6 +939,9 @@
       <c r="I10" s="3">
         <v>41507</v>
       </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -942,6 +969,9 @@
       </c>
       <c r="I11" s="3">
         <v>41507</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished code refactor into separate files
Also, added study GET allIds. See documentation on the Study endpoint
for details.
</commit_message>
<xml_diff>
--- a/test_files/ServiceTestMatrix.xlsx
+++ b/test_files/ServiceTestMatrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
   <si>
     <t>Endpoint</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>sessionId must be a valid ID (This changes with each session)</t>
+  </si>
+  <si>
+    <t>allIds</t>
+  </si>
+  <si>
+    <t>allIds=true</t>
   </si>
 </sst>
 </file>
@@ -253,10 +259,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -619,17 +625,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H10" sqref="H10:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="30.42578125" customWidth="1"/>
     <col min="6" max="7" width="43.42578125" customWidth="1"/>
-    <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -665,155 +672,152 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="5" t="str">
+        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+        <v>http://wlux.uw.edu/rbwatson/study.php?allIds=true</v>
+      </c>
+      <c r="G2" s="5" t="str">
+        <f>CONCATENATE("http://localhost/rbwatson/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+        <v>http://localhost/rbwatson/study.php?allIds=true</v>
+      </c>
+      <c r="H2" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I2" s="6">
+        <v>41577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+      <c r="F3" t="str">
+        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
         <v>http://wlux.uw.edu/rbwatson/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
       </c>
-      <c r="G2" t="str">
-        <f>CONCATENATE("http://localhost/rbwatson/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+      <c r="G3" t="str">
+        <f>CONCATENATE("http://localhost/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
         <v>http://localhost/rbwatson/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
       </c>
-      <c r="H2" s="3">
-        <v>41504</v>
-      </c>
-      <c r="I2" s="3">
-        <v>41507</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="H3" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I3" s="6">
+        <v>41577</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="str">
-        <f t="shared" ref="F3:F16" si="0">CONCATENATE("http://wlux.uw.edu/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
+      <c r="F4" s="3" t="str">
+        <f t="shared" ref="F4:F17" si="0">CONCATENATE("http://wlux.uw.edu/rbwatson/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
         <v>http://wlux.uw.edu/rbwatson/study.php</v>
       </c>
-      <c r="G3" s="4" t="str">
-        <f>CONCATENATE("http://localhost/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
+      <c r="G4" s="3" t="str">
+        <f>CONCATENATE("http://localhost/rbwatson/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
         <v>http://localhost/rbwatson/study.php</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="4" t="str">
+      <c r="F5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/study.php</v>
       </c>
-      <c r="G4" s="4" t="str">
-        <f t="shared" ref="G4:G16" si="1">CONCATENATE("http://localhost/rbwatson/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
+      <c r="G5" s="3" t="str">
+        <f t="shared" ref="G5:G17" si="1">CONCATENATE("http://localhost/rbwatson/",A5,".php", IF(D5&lt;&gt;"","?",""),D5)</f>
         <v>http://localhost/rbwatson/study.php</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A5,".php", IF(D5&lt;&gt;"","?",""),D5)</f>
+      <c r="F6" t="str">
+        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A6,".php", IF(D6&lt;&gt;"","?",""),D6)</f>
         <v>http://wlux.uw.edu/rbwatson/session.php</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G6" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/session.php</v>
       </c>
-      <c r="H5" s="3">
-        <v>41504</v>
-      </c>
-      <c r="I5" s="3">
-        <v>41507</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/task.php</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/task.php</v>
-      </c>
-      <c r="H6" s="3">
-        <v>41504</v>
-      </c>
-      <c r="I6" s="3">
-        <v>41507</v>
+      <c r="H6" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I6" s="6">
+        <v>41577</v>
       </c>
       <c r="J6" t="s">
         <v>32</v>
@@ -827,10 +831,10 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -840,11 +844,11 @@
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/task.php</v>
       </c>
-      <c r="H7" s="3">
-        <v>41504</v>
-      </c>
-      <c r="I7" s="3">
-        <v>41507</v>
+      <c r="H7" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I7" s="6">
+        <v>41577</v>
       </c>
       <c r="J7" t="s">
         <v>32</v>
@@ -852,7 +856,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -861,21 +865,21 @@
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/session.php</v>
+        <v>http://wlux.uw.edu/rbwatson/task.php</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/session.php</v>
-      </c>
-      <c r="H8" s="3">
-        <v>41504</v>
-      </c>
-      <c r="I8" s="3">
-        <v>41507</v>
+        <v>http://localhost/rbwatson/task.php</v>
+      </c>
+      <c r="H8" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I8" s="6">
+        <v>41577</v>
       </c>
       <c r="J8" t="s">
         <v>32</v>
@@ -886,208 +890,239 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
+        <v>http://wlux.uw.edu/rbwatson/session.php</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>41506</v>
-      </c>
-      <c r="I9" s="3">
-        <v>41507</v>
+        <v>http://localhost/rbwatson/session.php</v>
+      </c>
+      <c r="H9" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I9" s="6">
+        <v>41577</v>
       </c>
       <c r="J9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I10" s="6">
+        <v>41577</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="6" t="str">
+      <c r="F11" s="5" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="G10" s="6" t="str">
+      <c r="G11" s="5" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="H10" s="3">
-        <v>41506</v>
-      </c>
-      <c r="I10" s="3">
-        <v>41507</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="H11" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I11" s="6">
+        <v>41577</v>
+      </c>
+      <c r="J11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="6" t="str">
+      <c r="F12" s="5" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="G11" s="6" t="str">
+      <c r="G12" s="5" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
-      <c r="H11" s="3">
-        <v>41506</v>
-      </c>
-      <c r="I11" s="3">
-        <v>41507</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="H12" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I12" s="6">
+        <v>41577</v>
+      </c>
+      <c r="J12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="str">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/log.php</v>
       </c>
-      <c r="G12" s="4" t="str">
+      <c r="G13" s="3" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/log.php</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="str">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/log.php</v>
       </c>
-      <c r="G13" s="4" t="str">
+      <c r="G14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/log.php</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="str">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/log.php</v>
       </c>
-      <c r="G14" s="4" t="str">
+      <c r="G15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/log.php</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="str">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/log.php</v>
       </c>
-      <c r="G15" s="4" t="str">
+      <c r="G16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/log.php</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="str">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/rbwatson/log.php</v>
       </c>
-      <c r="G16" s="4" t="str">
+      <c r="G17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>http://localhost/rbwatson/log.php</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Big refactor to make the folder structure a little more sensible
See the readme.md for details.
</commit_message>
<xml_diff>
--- a/test_files/ServiceTestMatrix.xlsx
+++ b/test_files/ServiceTestMatrix.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="5460" windowWidth="25485" windowHeight="11160" tabRatio="318"/>
+    <workbookView xWindow="1820" yWindow="5460" windowWidth="25480" windowHeight="11160" tabRatio="318"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -68,9 +68,6 @@
     <t>PUT</t>
   </si>
   <si>
-    <t>{"data":{"studyId":"1235","sessionId":"0","taskId":"1","conditionId":"4","conditionCssUrl":"css/style4.css","taskBarCssUrl":"http://localhost/rbwatson/wluxTaskBar.css","startUrl":"http://students.washington.edu/rbwatson/hearts.html","returnUrl":"http://localhost/rbwatson/end.php","buttonText":"End task","tabShowText":"Show","tabHideText":"Hide","taskText":"This is the task to do.","taskHtml":null}}</t>
-  </si>
-  <si>
     <t>{"data":{"studyId":"1235","sessionId":"0","taskId":"1","conditionId":"4","buttonText":"End task NOW!"}}</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>allIds=true</t>
+  </si>
+  <si>
+    <t>{"data":{"studyId":"1235","sessionId":"0","taskId":"1","conditionId":"4","conditionCssUrl":"css/style4.css","taskBarCssUrl":"http://localhost/data/wluxTaskBar.css","startUrl":"http://students.washington.edu/data/hearts.html","returnUrl":"http://localhost/data/end.php","buttonText":"End task","tabShowText":"Show","tabHideText":"Hide","taskText":"This is the task to do.","taskHtml":null}}</t>
   </si>
 </sst>
 </file>
@@ -194,8 +194,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -264,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -293,6 +297,8 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -321,6 +327,8 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -627,20 +635,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="7" width="43.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="44.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.5" customWidth="1"/>
+    <col min="6" max="7" width="43.5" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="29.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,10 +677,10 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -680,18 +688,18 @@
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" s="5" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
-        <v>http://wlux.uw.edu/rbwatson/study.php?allIds=true</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+        <v>http://wlux.uw.edu/data/study.php?allIds=true</v>
       </c>
       <c r="G2" s="5" t="str">
-        <f>CONCATENATE("http://localhost/rbwatson/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
-        <v>http://localhost/rbwatson/study.php?allIds=true</v>
+        <f>CONCATENATE("http://localhost/data/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+        <v>http://localhost/data/study.php?allIds=true</v>
       </c>
       <c r="H2" s="6">
         <v>41577</v>
@@ -700,7 +708,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -708,18 +716,18 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
-        <v>http://wlux.uw.edu/rbwatson/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
+        <v>http://wlux.uw.edu/data/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
       </c>
       <c r="G3" t="str">
-        <f>CONCATENATE("http://localhost/rbwatson/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
-        <v>http://localhost/rbwatson/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
+        <f>CONCATENATE("http://localhost/data/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
+        <v>http://localhost/data/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
       </c>
       <c r="H3" s="6">
         <v>41577</v>
@@ -728,7 +736,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -736,19 +744,19 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f t="shared" ref="F4:F17" si="0">CONCATENATE("http://wlux.uw.edu/rbwatson/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
-        <v>http://wlux.uw.edu/rbwatson/study.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
+        <v>http://wlux.uw.edu/data/study.php</v>
       </c>
       <c r="G4" s="3" t="str">
-        <f>CONCATENATE("http://localhost/rbwatson/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
-        <v>http://localhost/rbwatson/study.php</v>
+        <f>CONCATENATE("http://localhost/data/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
+        <v>http://localhost/data/study.php</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>13</v>
@@ -757,10 +765,10 @@
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -768,19 +776,19 @@
         <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/study.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A5,".php", IF(D5&lt;&gt;"","?",""),D5)</f>
+        <v>http://wlux.uw.edu/data/study.php</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f t="shared" ref="G5:G17" si="1">CONCATENATE("http://localhost/rbwatson/",A5,".php", IF(D5&lt;&gt;"","?",""),D5)</f>
-        <v>http://localhost/rbwatson/study.php</v>
+        <f>CONCATENATE("http://localhost/data/",A5,".php", IF(D5&lt;&gt;"","?",""),D5)</f>
+        <v>http://localhost/data/study.php</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>13</v>
@@ -789,29 +797,29 @@
         <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
       <c r="F6" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/rbwatson/",A6,".php", IF(D6&lt;&gt;"","?",""),D6)</f>
-        <v>http://wlux.uw.edu/rbwatson/session.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A6,".php", IF(D6&lt;&gt;"","?",""),D6)</f>
+        <v>http://wlux.uw.edu/data/session.php</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/session.php</v>
+        <f>CONCATENATE("http://localhost/data/",A6,".php", IF(D6&lt;&gt;"","?",""),D6)</f>
+        <v>http://localhost/data/session.php</v>
       </c>
       <c r="H6" s="6">
         <v>41577</v>
@@ -820,29 +828,29 @@
         <v>41577</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/task.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A7,".php", IF(D7&lt;&gt;"","?",""),D7)</f>
+        <v>http://wlux.uw.edu/data/task.php</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/task.php</v>
+        <f>CONCATENATE("http://localhost/data/",A7,".php", IF(D7&lt;&gt;"","?",""),D7)</f>
+        <v>http://localhost/data/task.php</v>
       </c>
       <c r="H7" s="6">
         <v>41577</v>
@@ -851,29 +859,29 @@
         <v>41577</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/task.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A8,".php", IF(D8&lt;&gt;"","?",""),D8)</f>
+        <v>http://wlux.uw.edu/data/task.php</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/task.php</v>
+        <f>CONCATENATE("http://localhost/data/",A8,".php", IF(D8&lt;&gt;"","?",""),D8)</f>
+        <v>http://localhost/data/task.php</v>
       </c>
       <c r="H8" s="6">
         <v>41577</v>
@@ -882,29 +890,29 @@
         <v>41577</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
       <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/session.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A9,".php", IF(D9&lt;&gt;"","?",""),D9)</f>
+        <v>http://wlux.uw.edu/data/session.php</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/session.php</v>
+        <f>CONCATENATE("http://localhost/data/",A9,".php", IF(D9&lt;&gt;"","?",""),D9)</f>
+        <v>http://localhost/data/session.php</v>
       </c>
       <c r="H9" s="6">
         <v>41577</v>
@@ -913,29 +921,29 @@
         <v>41577</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A10,".php", IF(D10&lt;&gt;"","?",""),D10)</f>
+        <v>http://wlux.uw.edu/data/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
+        <f>CONCATENATE("http://localhost/data/",A10,".php", IF(D10&lt;&gt;"","?",""),D10)</f>
+        <v>http://localhost/data/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
       </c>
       <c r="H10" s="6">
         <v>41577</v>
@@ -944,60 +952,60 @@
         <v>41577</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="5" customFormat="1">
       <c r="A11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="5" t="str">
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A11,".php", IF(D11&lt;&gt;"","?",""),D11)</f>
+        <v>http://wlux.uw.edu/data/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+      </c>
+      <c r="G11" s="5" t="str">
+        <f>CONCATENATE("http://localhost/data/",A11,".php", IF(D11&lt;&gt;"","?",""),D11)</f>
+        <v>http://localhost/data/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>41577</v>
+      </c>
+      <c r="I11" s="6">
+        <v>41577</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="5" customFormat="1">
+      <c r="A12" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
-      </c>
-      <c r="G11" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
-      </c>
-      <c r="H11" s="6">
-        <v>41577</v>
-      </c>
-      <c r="I11" s="6">
-        <v>41577</v>
-      </c>
-      <c r="J11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A12,".php", IF(D12&lt;&gt;"","?",""),D12)</f>
+        <v>http://wlux.uw.edu/data/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
       <c r="G12" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
+        <f>CONCATENATE("http://localhost/data/",A12,".php", IF(D12&lt;&gt;"","?",""),D12)</f>
+        <v>http://localhost/data/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
       <c r="H12" s="6">
         <v>41577</v>
@@ -1006,58 +1014,58 @@
         <v>41577</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A13,".php", IF(D13&lt;&gt;"","?",""),D13)</f>
+        <v>http://wlux.uw.edu/data/log.php</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/log.php</v>
+        <f>CONCATENATE("http://localhost/data/",A13,".php", IF(D13&lt;&gt;"","?",""),D13)</f>
+        <v>http://localhost/data/log.php</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A14,".php", IF(D14&lt;&gt;"","?",""),D14)</f>
+        <v>http://wlux.uw.edu/data/log.php</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/log.php</v>
+        <f>CONCATENATE("http://localhost/data/",A14,".php", IF(D14&lt;&gt;"","?",""),D14)</f>
+        <v>http://localhost/data/log.php</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
@@ -1068,65 +1076,65 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A15,".php", IF(D15&lt;&gt;"","?",""),D15)</f>
+        <v>http://wlux.uw.edu/data/log.php</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/log.php</v>
+        <f>CONCATENATE("http://localhost/data/",A15,".php", IF(D15&lt;&gt;"","?",""),D15)</f>
+        <v>http://localhost/data/log.php</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A16,".php", IF(D16&lt;&gt;"","?",""),D16)</f>
+        <v>http://wlux.uw.edu/data/log.php</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/log.php</v>
+        <f>CONCATENATE("http://localhost/data/",A16,".php", IF(D16&lt;&gt;"","?",""),D16)</f>
+        <v>http://localhost/data/log.php</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wlux.uw.edu/rbwatson/log.php</v>
+        <f>CONCATENATE("http://wlux.uw.edu/data/",A17,".php", IF(D17&lt;&gt;"","?",""),D17)</f>
+        <v>http://wlux.uw.edu/data/log.php</v>
       </c>
       <c r="G17" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>http://localhost/rbwatson/log.php</v>
+        <f>CONCATENATE("http://localhost/data/",A17,".php", IF(D17&lt;&gt;"","?",""),D17)</f>
+        <v>http://localhost/data/log.php</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1141,7 +1149,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1158,7 +1166,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated table to include new Log function tests
</commit_message>
<xml_diff>
--- a/test_files/ServiceTestMatrix.xlsx
+++ b/test_files/ServiceTestMatrix.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="5460" windowWidth="25480" windowHeight="11160" tabRatio="318"/>
+    <workbookView xWindow="1815" yWindow="5460" windowWidth="25485" windowHeight="11160" tabRatio="318"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t>Endpoint</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>{"data":{"studyId":"1235","sessionId":"0","taskId":"1","conditionId":"4","conditionCssUrl":"css/style4.css","taskBarCssUrl":"http://localhost/data/wluxTaskBar.css","startUrl":"http://students.washington.edu/data/hearts.html","returnUrl":"http://localhost/data/end.php","buttonText":"End task","tabShowText":"Show","tabHideText":"Hide","taskText":"This is the task to do.","taskHtml":null}}</t>
+  </si>
+  <si>
+    <t>studyId=1234</t>
+  </si>
+  <si>
+    <t>sessionId=1383605381</t>
+  </si>
+  <si>
+    <t>sessionId=1383605381&amp;taskId=1</t>
   </si>
 </sst>
 </file>
@@ -635,20 +644,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
-    <col min="6" max="7" width="43.5" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="44.5" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="7" width="43.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.25" customHeight="1">
+    <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1">
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -694,11 +703,11 @@
         <v>33</v>
       </c>
       <c r="F2" s="5" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+        <f t="shared" ref="F2:F17" si="0">CONCATENATE("http://wlux.uw.edu/data/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
         <v>http://wlux.uw.edu/data/study.php?allIds=true</v>
       </c>
       <c r="G2" s="5" t="str">
-        <f>CONCATENATE("http://localhost/data/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
+        <f t="shared" ref="G2:G17" si="1">CONCATENATE("http://localhost/data/",A2,".php", IF(D2&lt;&gt;"","?",""),D2)</f>
         <v>http://localhost/data/study.php?allIds=true</v>
       </c>
       <c r="H2" s="6">
@@ -708,7 +717,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -726,7 +735,7 @@
         <v>http://wlux.uw.edu/data/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
       </c>
       <c r="G3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A3,".php", IF(D3&lt;&gt;"","?",""),D3)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/study.php?config[studyId]=1234&amp;config[conditionId]=4&amp;config[taskId]=1</v>
       </c>
       <c r="H3" s="6">
@@ -736,7 +745,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -751,11 +760,11 @@
         <v>34</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/study.php</v>
       </c>
       <c r="G4" s="3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A4,".php", IF(D4&lt;&gt;"","?",""),D4)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/study.php</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -768,7 +777,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -783,11 +792,11 @@
         <v>15</v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A5,".php", IF(D5&lt;&gt;"","?",""),D5)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/study.php</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A5,".php", IF(D5&lt;&gt;"","?",""),D5)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/study.php</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -800,7 +809,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -814,11 +823,11 @@
         <v>18</v>
       </c>
       <c r="F6" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A6,".php", IF(D6&lt;&gt;"","?",""),D6)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/session.php</v>
       </c>
       <c r="G6" t="str">
-        <f>CONCATENATE("http://localhost/data/",A6,".php", IF(D6&lt;&gt;"","?",""),D6)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/session.php</v>
       </c>
       <c r="H6" s="6">
@@ -831,7 +840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -845,11 +854,11 @@
         <v>21</v>
       </c>
       <c r="F7" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A7,".php", IF(D7&lt;&gt;"","?",""),D7)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/task.php</v>
       </c>
       <c r="G7" t="str">
-        <f>CONCATENATE("http://localhost/data/",A7,".php", IF(D7&lt;&gt;"","?",""),D7)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/task.php</v>
       </c>
       <c r="H7" s="6">
@@ -862,7 +871,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -876,11 +885,11 @@
         <v>24</v>
       </c>
       <c r="F8" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A8,".php", IF(D8&lt;&gt;"","?",""),D8)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/task.php</v>
       </c>
       <c r="G8" t="str">
-        <f>CONCATENATE("http://localhost/data/",A8,".php", IF(D8&lt;&gt;"","?",""),D8)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/task.php</v>
       </c>
       <c r="H8" s="6">
@@ -893,7 +902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -907,11 +916,11 @@
         <v>23</v>
       </c>
       <c r="F9" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A9,".php", IF(D9&lt;&gt;"","?",""),D9)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/session.php</v>
       </c>
       <c r="G9" t="str">
-        <f>CONCATENATE("http://localhost/data/",A9,".php", IF(D9&lt;&gt;"","?",""),D9)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/session.php</v>
       </c>
       <c r="H9" s="6">
@@ -924,7 +933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -938,11 +947,11 @@
         <v>26</v>
       </c>
       <c r="F10" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A10,".php", IF(D10&lt;&gt;"","?",""),D10)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
       </c>
       <c r="G10" t="str">
-        <f>CONCATENATE("http://localhost/data/",A10,".php", IF(D10&lt;&gt;"","?",""),D10)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/session.php?log[sessionId]=1377057169&amp;log[conditionId]=3&amp;log[taskId]=0</v>
       </c>
       <c r="H10" s="6">
@@ -955,7 +964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="5" customFormat="1">
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -969,11 +978,11 @@
         <v>27</v>
       </c>
       <c r="F11" s="5" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A11,".php", IF(D11&lt;&gt;"","?",""),D11)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
       <c r="G11" s="5" t="str">
-        <f>CONCATENATE("http://localhost/data/",A11,".php", IF(D11&lt;&gt;"","?",""),D11)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/session.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
       <c r="H11" s="6">
@@ -986,7 +995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="5" customFormat="1">
+    <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -1000,11 +1009,11 @@
         <v>27</v>
       </c>
       <c r="F12" s="5" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A12,".php", IF(D12&lt;&gt;"","?",""),D12)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
       <c r="G12" s="5" t="str">
-        <f>CONCATENATE("http://localhost/data/",A12,".php", IF(D12&lt;&gt;"","?",""),D12)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/task.php?config[sessionId]=1377058693&amp;config[taskId]=1</v>
       </c>
       <c r="H12" s="6">
@@ -1017,7 +1026,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -1030,17 +1039,17 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A13,".php", IF(D13&lt;&gt;"","?",""),D13)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/log.php</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A13,".php", IF(D13&lt;&gt;"","?",""),D13)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/log.php</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1053,84 +1062,81 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A14,".php", IF(D14&lt;&gt;"","?",""),D14)</f>
+        <f t="shared" si="0"/>
         <v>http://wlux.uw.edu/data/log.php</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A14,".php", IF(D14&lt;&gt;"","?",""),D14)</f>
+        <f t="shared" si="1"/>
         <v>http://localhost/data/log.php</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A15,".php", IF(D15&lt;&gt;"","?",""),D15)</f>
-        <v>http://wlux.uw.edu/data/log.php</v>
-      </c>
-      <c r="G15" s="3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A15,".php", IF(D15&lt;&gt;"","?",""),D15)</f>
-        <v>http://localhost/data/log.php</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="3" t="s">
+      <c r="D15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/data/log.php?studyId=1234</v>
+      </c>
+      <c r="G15" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/data/log.php?studyId=1234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A16,".php", IF(D16&lt;&gt;"","?",""),D16)</f>
-        <v>http://wlux.uw.edu/data/log.php</v>
-      </c>
-      <c r="G16" s="3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A16,".php", IF(D16&lt;&gt;"","?",""),D16)</f>
-        <v>http://localhost/data/log.php</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="3" t="s">
+      <c r="D16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/data/log.php?sessionId=1383605381</v>
+      </c>
+      <c r="G16" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/data/log.php?sessionId=1383605381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="str">
-        <f>CONCATENATE("http://wlux.uw.edu/data/",A17,".php", IF(D17&lt;&gt;"","?",""),D17)</f>
-        <v>http://wlux.uw.edu/data/log.php</v>
-      </c>
-      <c r="G17" s="3" t="str">
-        <f>CONCATENATE("http://localhost/data/",A17,".php", IF(D17&lt;&gt;"","?",""),D17)</f>
-        <v>http://localhost/data/log.php</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="D17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>http://wlux.uw.edu/data/log.php?sessionId=1383605381&amp;taskId=1</v>
+      </c>
+      <c r="G17" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>http://localhost/data/log.php?sessionId=1383605381&amp;taskId=1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1149,7 +1155,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1166,7 +1172,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>